<commit_message>
Terminado tema de AE
</commit_message>
<xml_diff>
--- a/Clases/AG_10-25-2023.xlsx
+++ b/Clases/AG_10-25-2023.xlsx
@@ -8,102 +8,135 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Metodos\Clases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF8CE02-2BB6-4A3B-A600-73CA2B4AC4B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BCCEE8-972A-4771-9840-EF091B35ADBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{A56C292F-9C71-4E43-88C6-7084E961FE8A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="6" xr2:uid="{A56C292F-9C71-4E43-88C6-7084E961FE8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Ejercicio 1" sheetId="1" r:id="rId1"/>
     <sheet name="Answer Report 1" sheetId="7" r:id="rId2"/>
     <sheet name="Population Report 1" sheetId="8" r:id="rId3"/>
-    <sheet name="Ejercicio 2 AE" sheetId="6" r:id="rId4"/>
-    <sheet name="Sheet9" sheetId="9" r:id="rId5"/>
+    <sheet name="Answer Report 2" sheetId="13" r:id="rId4"/>
+    <sheet name="Population Report 2" sheetId="14" r:id="rId5"/>
+    <sheet name="Ejercicio 2 AE" sheetId="6" r:id="rId6"/>
+    <sheet name="Ejercicio 2 NA" sheetId="9" r:id="rId7"/>
+    <sheet name="Ejercicio 2 GRG" sheetId="10" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">'Ejercicio 1'!$G$2:$H$2</definedName>
-    <definedName name="solver_adj" localSheetId="3" hidden="1">'Ejercicio 2 AE'!$F$3:$G$3</definedName>
+    <definedName name="solver_adj" localSheetId="5" hidden="1">'Ejercicio 2 AE'!$F$3:$G$3</definedName>
+    <definedName name="solver_adj" localSheetId="7" hidden="1">'Ejercicio 2 GRG'!$D$3:$E$3</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
-    <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="5" hidden="1">0.1</definedName>
+    <definedName name="solver_cvg" localSheetId="7" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="7" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_eng" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_eng" localSheetId="5" hidden="1">3</definedName>
+    <definedName name="solver_eng" localSheetId="7" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="7" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="7" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Ejercicio 1'!$F$3:$F$4</definedName>
-    <definedName name="solver_lhs1" localSheetId="3" hidden="1">'Ejercicio 2 AE'!$E$4:$E$5</definedName>
+    <definedName name="solver_lhs1" localSheetId="5" hidden="1">'Ejercicio 2 AE'!$E$4:$E$5</definedName>
+    <definedName name="solver_lhs1" localSheetId="7" hidden="1">'Ejercicio 2 GRG'!$C$4:$C$5</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Ejercicio 1'!$G$2</definedName>
-    <definedName name="solver_lhs2" localSheetId="3" hidden="1">'Ejercicio 2 AE'!$F$3</definedName>
+    <definedName name="solver_lhs2" localSheetId="5" hidden="1">'Ejercicio 2 AE'!$F$3</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">'Ejercicio 1'!$G$2</definedName>
-    <definedName name="solver_lhs3" localSheetId="3" hidden="1">'Ejercicio 2 AE'!$F$3</definedName>
+    <definedName name="solver_lhs3" localSheetId="5" hidden="1">'Ejercicio 2 AE'!$F$3</definedName>
     <definedName name="solver_lhs4" localSheetId="0" hidden="1">'Ejercicio 1'!$H$2</definedName>
-    <definedName name="solver_lhs4" localSheetId="3" hidden="1">'Ejercicio 2 AE'!$G$3</definedName>
+    <definedName name="solver_lhs4" localSheetId="5" hidden="1">'Ejercicio 2 AE'!$G$3</definedName>
     <definedName name="solver_lhs5" localSheetId="0" hidden="1">'Ejercicio 1'!$H$2</definedName>
-    <definedName name="solver_lhs5" localSheetId="3" hidden="1">'Ejercicio 2 AE'!$G$3</definedName>
+    <definedName name="solver_lhs5" localSheetId="5" hidden="1">'Ejercicio 2 AE'!$G$3</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="7" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="5" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="7" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.02</definedName>
-    <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="5" hidden="1">0.05</definedName>
+    <definedName name="solver_mrt" localSheetId="7" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="7" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="7" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="7" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">5</definedName>
-    <definedName name="solver_num" localSheetId="3" hidden="1">5</definedName>
+    <definedName name="solver_num" localSheetId="5" hidden="1">5</definedName>
+    <definedName name="solver_num" localSheetId="7" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="7" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">'Ejercicio 1'!$F$2</definedName>
-    <definedName name="solver_opt" localSheetId="3" hidden="1">'Ejercicio 2 AE'!$E$3</definedName>
+    <definedName name="solver_opt" localSheetId="5" hidden="1">'Ejercicio 2 AE'!$E$3</definedName>
+    <definedName name="solver_opt" localSheetId="7" hidden="1">'Ejercicio 2 GRG'!$C$3</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
-    <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="5" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="7" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="7" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="7" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel2" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel3" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="5" hidden="1">3</definedName>
     <definedName name="solver_rel4" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel4" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_rel5" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel5" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_rel5" localSheetId="5" hidden="1">3</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">'Ejercicio 1'!$G$3:$G$4</definedName>
-    <definedName name="solver_rhs1" localSheetId="3" hidden="1">'Ejercicio 2 AE'!$F$4:$F$5</definedName>
+    <definedName name="solver_rhs1" localSheetId="5" hidden="1">'Ejercicio 2 AE'!$F$4:$F$5</definedName>
+    <definedName name="solver_rhs1" localSheetId="7" hidden="1">'Ejercicio 2 GRG'!$D$4:$D$5</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">'Ejercicio 1'!$C$5</definedName>
-    <definedName name="solver_rhs2" localSheetId="3" hidden="1">'Ejercicio 2 AE'!$B$4</definedName>
+    <definedName name="solver_rhs2" localSheetId="5" hidden="1">'Ejercicio 2 AE'!$B$4</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">'Ejercicio 1'!$C$6</definedName>
-    <definedName name="solver_rhs3" localSheetId="3" hidden="1">'Ejercicio 2 AE'!$B$6</definedName>
+    <definedName name="solver_rhs3" localSheetId="5" hidden="1">'Ejercicio 2 AE'!$B$6</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">'Ejercicio 1'!$D$4</definedName>
-    <definedName name="solver_rhs4" localSheetId="3" hidden="1">'Ejercicio 2 AE'!$C$5</definedName>
+    <definedName name="solver_rhs4" localSheetId="5" hidden="1">'Ejercicio 2 AE'!$C$5</definedName>
     <definedName name="solver_rhs5" localSheetId="0" hidden="1">'Ejercicio 1'!$D$7</definedName>
-    <definedName name="solver_rhs5" localSheetId="3" hidden="1">'Ejercicio 2 AE'!$C$7</definedName>
+    <definedName name="solver_rhs5" localSheetId="5" hidden="1">'Ejercicio 2 AE'!$C$7</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="7" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="7" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_scl" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="7" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="7" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">10</definedName>
-    <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="5" hidden="1">1000000</definedName>
+    <definedName name="solver_ssz" localSheetId="7" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="7" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
-    <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="5" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="7" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_typ" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="7" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="7" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="5" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="7" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -126,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="87">
   <si>
     <t>Max Z =x+2y</t>
   </si>
@@ -357,6 +390,36 @@
   </si>
   <si>
     <t>Global</t>
+  </si>
+  <si>
+    <t>Parametros</t>
+  </si>
+  <si>
+    <t>100 individuos, 7.5% de mutacion 0.0001 de convergencia</t>
+  </si>
+  <si>
+    <t>Worksheet: [AG_10-25-2023.xlsx]Ejercicio 2 AE</t>
+  </si>
+  <si>
+    <t>5000 individuos, 20% de mutacion, 14134 poblaciones y 0.00001 de convergencia</t>
+  </si>
+  <si>
+    <t>Report Created: 10/26/2023 12:23:20 PM</t>
+  </si>
+  <si>
+    <t>Solution Time: 47 Seconds.</t>
+  </si>
+  <si>
+    <t>Iterations: 0 Subproblems: 14400</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Convergence 0.001, Population Size 10000, Random Seed 0, Mutation Rate 0.05, Time w/o Improve 30 sec, Require Bounds</t>
+  </si>
+  <si>
+    <t>10000 individuos, 5% de mutacion, 14400 poblaciones 0.001 de convergencia</t>
+  </si>
+  <si>
+    <t>Max Z =x^2+3y</t>
   </si>
 </sst>
 </file>
@@ -481,7 +544,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -506,6 +569,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -823,7 +900,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A5"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1476,120 +1553,317 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA718AB-0EEF-423C-B8A0-FEFF487467AA}">
-  <dimension ref="A1:G7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EA6EE7C-01E7-44D9-86BC-95BAF44D8CE1}">
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="10">
-        <f>F3^2+2*G3</f>
-        <v>99.999337119833328</v>
-      </c>
-      <c r="F3" s="10">
-        <v>9.9999668429711335</v>
-      </c>
-      <c r="G3" s="10">
-        <v>1.2965563504050274E-7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="10">
-        <f>35/2</f>
-        <v>17.5</v>
-      </c>
-      <c r="C4" s="10">
-        <f>35/4</f>
-        <v>8.75</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4">
-        <f>2*F3+4*G3</f>
-        <v>19.999934204564806</v>
-      </c>
-      <c r="F4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="10">
-        <f>30/3</f>
-        <v>10</v>
-      </c>
-      <c r="C5" s="10">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5">
-        <f>3*F3+2*G3</f>
-        <v>29.999900788224672</v>
-      </c>
-      <c r="F5">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="17">
+        <v>0</v>
+      </c>
+      <c r="E16" s="17">
+        <v>99.741484367970259</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="18">
+        <v>0</v>
+      </c>
+      <c r="E21" s="18">
+        <v>9.9853502586217733</v>
+      </c>
+      <c r="F21" s="16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="10">
-        <v>0</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="10">
-        <v>0</v>
+    <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="17">
+        <v>0</v>
+      </c>
+      <c r="E22" s="17">
+        <v>1.7132290306172977E-2</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B27" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="18">
+        <v>20.039229678468239</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G27" s="16">
+        <v>14.960770321531761</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="18">
+        <v>29.990315356477666</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G28" s="16">
+        <v>9.6846435223341132E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B29" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="18">
+        <v>9.9853502586217733</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G29" s="16">
+        <v>7.5146497413782267</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B30" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="18">
+        <v>9.9853502586217733</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G30" s="18">
+        <v>9.9853502586217733</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B31" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="18">
+        <v>1.7132290306172977E-2</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G31" s="16">
+        <v>14.982867709693828</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D32" s="17">
+        <v>1.7132290306172977E-2</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G32" s="17">
+        <v>1.7132290306172977E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1598,11 +1872,403 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6BF51FB-1FC1-4C3E-8ADA-D140A49FCFD0}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="18">
+        <v>9.9853502586217733</v>
+      </c>
+      <c r="E9" s="18">
+        <v>6.4840511661875597</v>
+      </c>
+      <c r="F9" s="16">
+        <v>2.3264140569633369</v>
+      </c>
+      <c r="G9" s="16">
+        <v>9.9853502586217733</v>
+      </c>
+      <c r="H9" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="17">
+        <v>1.7132290306172977E-2</v>
+      </c>
+      <c r="E10" s="17">
+        <v>2.6170623474485546</v>
+      </c>
+      <c r="F10" s="14">
+        <v>1.6204222323703228</v>
+      </c>
+      <c r="G10" s="14">
+        <v>8.7086710630490778</v>
+      </c>
+      <c r="H10" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="18">
+        <v>20.039229678468239</v>
+      </c>
+      <c r="E15" s="18">
+        <v>23.436351722169434</v>
+      </c>
+      <c r="F15" s="16">
+        <v>6.0534198873652514</v>
+      </c>
+      <c r="G15" s="16">
+        <v>34.989330418081103</v>
+      </c>
+      <c r="H15" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="17">
+        <v>29.990315356477666</v>
+      </c>
+      <c r="E16" s="17">
+        <v>24.686278193459898</v>
+      </c>
+      <c r="F16" s="14">
+        <v>6.2409925289893922</v>
+      </c>
+      <c r="G16" s="14">
+        <v>29.997486675855466</v>
+      </c>
+      <c r="H16" s="14">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA718AB-0EEF-423C-B8A0-FEFF487467AA}">
+  <dimension ref="A1:M7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="68.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="10">
+        <f>F3^2+2*G3</f>
+        <v>98.399689995136256</v>
+      </c>
+      <c r="F3" s="10">
+        <v>9.9071615235447705</v>
+      </c>
+      <c r="G3" s="10">
+        <v>0.12392027076516314</v>
+      </c>
+      <c r="J3" s="10">
+        <v>99.999337119833328</v>
+      </c>
+      <c r="K3" s="10">
+        <v>9.9999668429711335</v>
+      </c>
+      <c r="L3" s="10">
+        <v>1.2965563504050274E-7</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="10">
+        <f>35/2</f>
+        <v>17.5</v>
+      </c>
+      <c r="C4" s="10">
+        <f>35/4</f>
+        <v>8.75</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <f>2*F3+4*G3</f>
+        <v>20.310004130150194</v>
+      </c>
+      <c r="F4">
+        <v>35</v>
+      </c>
+      <c r="J4" s="10">
+        <v>99.963227493578643</v>
+      </c>
+      <c r="K4" s="10">
+        <v>9.9981612056206934</v>
+      </c>
+      <c r="L4" s="10">
+        <v>0</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="10">
+        <f>30/3</f>
+        <v>10</v>
+      </c>
+      <c r="C5" s="10">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <f>3*F3+2*G3</f>
+        <v>29.969325112164636</v>
+      </c>
+      <c r="F5">
+        <v>30</v>
+      </c>
+      <c r="J5">
+        <v>99.845628534522461</v>
+      </c>
+      <c r="K5">
+        <v>9.9918084276871859</v>
+      </c>
+      <c r="L5">
+        <v>4.6964394608914901E-3</v>
+      </c>
+      <c r="M5" s="21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="10">
+        <v>0</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA2B424-AE82-4EA8-8E0A-64762CDFECCC}">
   <dimension ref="A1:T751"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1641,23 +2307,23 @@
       </c>
       <c r="O1">
         <f ca="1">MAX(L2:L101)</f>
-        <v>77.172703081199401</v>
+        <v>61.640534292419616</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" s="12">
         <f ca="1">RAND()*17.5</f>
-        <v>1.4115357330223435</v>
+        <v>7.1877375709912696</v>
       </c>
       <c r="G2">
         <f ca="1">RAND()*15</f>
-        <v>0.12571316399108134</v>
+        <v>0.85074883102669308</v>
       </c>
       <c r="H2">
         <f ca="1">IF(2*F2+4*G2&lt;=35,1,0)</f>
@@ -1668,15 +2334,15 @@
         <v>1</v>
       </c>
       <c r="L2" s="13">
-        <f ca="1">IF(H2*I2=1,F2^2+2*G2,"X")</f>
-        <v>2.243859453581087</v>
+        <f ca="1">IF(H2*I2=1,F2^2+3*G2,"X")</f>
+        <v>54.215817882519552</v>
       </c>
       <c r="N2" t="s">
         <v>6</v>
       </c>
       <c r="O2">
         <f ca="1">INDEX(F2:F101, MATCH(O1,L2:L101,0))</f>
-        <v>8.7596799154483413</v>
+        <v>7.4255091813766505</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
@@ -1694,11 +2360,11 @@
       </c>
       <c r="F3" s="12">
         <f t="shared" ref="F3:F66" ca="1" si="0">RAND()*17.5</f>
-        <v>2.0468771509206789</v>
+        <v>11.589919683232196</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G66" ca="1" si="1">RAND()*15</f>
-        <v>13.027734835915501</v>
+        <v>7.8250842090761479</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H66" ca="1" si="2">IF(2*F3+4*G3&lt;=35,1,0)</f>
@@ -1717,7 +2383,7 @@
       </c>
       <c r="O3">
         <f ca="1">INDEX(G2:G101, MATCH(O1,L2:L101,0))</f>
-        <v>0.22035543004516656</v>
+        <v>3.2511738448553427</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
@@ -1740,11 +2406,11 @@
       </c>
       <c r="F4" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2313538791378997</v>
+        <v>16.654623208051543</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="1"/>
-        <v>14.605529532785596</v>
+        <v>10.287905423421563</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="2"/>
@@ -1796,11 +2462,11 @@
       </c>
       <c r="F5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>9.3903993819938716</v>
+        <v>8.321035670123436</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="1"/>
-        <v>14.065151363669749</v>
+        <v>14.038185183233406</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="2"/>
@@ -1818,7 +2484,7 @@
         <v>70</v>
       </c>
       <c r="O5">
-        <v>89.840990929052268</v>
+        <v>96.840990929052296</v>
       </c>
       <c r="P5">
         <v>87.136026709003076</v>
@@ -1848,23 +2514,23 @@
       </c>
       <c r="F6" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11592154850546127</v>
+        <v>15.988900023607298</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="1"/>
-        <v>4.1411843108618198</v>
+        <v>3.9354735564107561</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L6" s="13">
+        <v>0</v>
+      </c>
+      <c r="L6" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>8.2958064271315433</v>
+        <v>X</v>
       </c>
       <c r="N6" t="s">
         <v>6</v>
@@ -1897,11 +2563,11 @@
       </c>
       <c r="F7" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0136935171586328</v>
+        <v>6.5745941444558467</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="1"/>
-        <v>6.9989641620830607</v>
+        <v>1.6031778442236226</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="2"/>
@@ -1913,7 +2579,7 @@
       </c>
       <c r="L7" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>18.052889905212826</v>
+        <v>46.431643852760352</v>
       </c>
       <c r="N7" t="s">
         <v>7</v>
@@ -1940,23 +2606,23 @@
       </c>
       <c r="F8" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5582232187208489</v>
+        <v>17.435517696570717</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="1"/>
-        <v>5.7352642434651688</v>
+        <v>14.894702013914268</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L8" s="13">
+        <v>0</v>
+      </c>
+      <c r="L8" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>11.782141648849402</v>
+        <v>X</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
@@ -1965,11 +2631,11 @@
       </c>
       <c r="F9" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>13.757969918038263</v>
+        <v>10.80244408276247</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="1"/>
-        <v>7.5615289580657254</v>
+        <v>7.8440314844306993</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="2"/>
@@ -1990,11 +2656,11 @@
       </c>
       <c r="F10" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>15.413611891087315</v>
+        <v>6.9140032533194455</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="1"/>
-        <v>12.503774639722446</v>
+        <v>11.803125234245227</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="2"/>
@@ -2015,15 +2681,15 @@
       </c>
       <c r="F11" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>16.069056551010817</v>
+        <v>10.027304944991956</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="1"/>
-        <v>13.654229813523598</v>
+        <v>1.9296957630308249</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="3"/>
@@ -2040,23 +2706,23 @@
       </c>
       <c r="F12" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>6.4020168846905161</v>
+        <v>7.4255091813766505</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="1"/>
-        <v>7.7098317748868723</v>
+        <v>3.2511738448553427</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L12" s="13" t="str">
+        <v>1</v>
+      </c>
+      <c r="L12" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>X</v>
+        <v>61.640534292419616</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
@@ -2065,15 +2731,15 @@
       </c>
       <c r="F13" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>4.8893737789770917</v>
+        <v>12.130734841371655</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="1"/>
-        <v>8.7453356641341351</v>
+        <v>1.7898493598848391</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="3"/>
@@ -2090,23 +2756,23 @@
       </c>
       <c r="F14" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5345520816528593</v>
+        <v>15.12828246742575</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="1"/>
-        <v>5.9524546503064215</v>
+        <v>12.499258091514264</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L14" s="13">
+        <v>0</v>
+      </c>
+      <c r="L14" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>24.397967718529404</v>
+        <v>X</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
@@ -2115,23 +2781,23 @@
       </c>
       <c r="F15" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>6.7594769345747574</v>
+        <v>12.925176856965633</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="1"/>
-        <v>1.121056377059479</v>
+        <v>9.4624116524500383</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L15" s="13">
+        <v>0</v>
+      </c>
+      <c r="L15" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>47.932641183167114</v>
+        <v>X</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
@@ -2140,11 +2806,11 @@
       </c>
       <c r="F16" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>9.5613123461674743</v>
+        <v>11.244055440664638</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="1"/>
-        <v>6.0838726251337096</v>
+        <v>8.1863293207284276</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="2"/>
@@ -2165,23 +2831,23 @@
       </c>
       <c r="F17" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>8.2628085597045686</v>
+        <v>7.0869116054819035</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="1"/>
-        <v>5.8475665648665061</v>
+        <v>0.5984965420452365</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L17" s="13" t="str">
+        <v>1</v>
+      </c>
+      <c r="L17" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>X</v>
+        <v>51.421309188004564</v>
       </c>
     </row>
     <row r="18" spans="5:12" x14ac:dyDescent="0.3">
@@ -2190,15 +2856,15 @@
       </c>
       <c r="F18" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>5.7243634573289857</v>
+        <v>9.9581214182573543</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="1"/>
-        <v>12.137630132775836</v>
+        <v>3.4474547854450899</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="3"/>
@@ -2215,11 +2881,11 @@
       </c>
       <c r="F19" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2553676727553944</v>
+        <v>11.82950065256775</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="1"/>
-        <v>13.140059613996266</v>
+        <v>9.0433054878794188</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="2"/>
@@ -2240,23 +2906,23 @@
       </c>
       <c r="F20" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>8.2039072609708068</v>
+        <v>16.742815129237435</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7006379140622196E-2</v>
+        <v>2.8094798723887626</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L20" s="13">
+        <v>0</v>
+      </c>
+      <c r="L20" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>67.338107104890781</v>
+        <v>X</v>
       </c>
     </row>
     <row r="21" spans="5:12" x14ac:dyDescent="0.3">
@@ -2265,23 +2931,23 @@
       </c>
       <c r="F21" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>7.5053742882791283</v>
+        <v>15.592726053716095</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.74733793081467048</v>
+        <v>10.196101533015971</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L21" s="13">
+        <v>0</v>
+      </c>
+      <c r="L21" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>57.825319068790769</v>
+        <v>X</v>
       </c>
     </row>
     <row r="22" spans="5:12" x14ac:dyDescent="0.3">
@@ -2290,11 +2956,11 @@
       </c>
       <c r="F22" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>10.242823159422244</v>
+        <v>10.390221943518176</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="1"/>
-        <v>10.585962531304794</v>
+        <v>13.261641145914997</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="2"/>
@@ -2315,11 +2981,11 @@
       </c>
       <c r="F23" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>13.381782280084876</v>
+        <v>9.1279344636749364</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="1"/>
-        <v>13.222719369094685</v>
+        <v>8.4922360076873886</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="2"/>
@@ -2340,11 +3006,11 @@
       </c>
       <c r="F24" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>5.2534914402510846E-2</v>
+        <v>1.733439442898346</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="1"/>
-        <v>8.2402686884429581</v>
+        <v>3.7362353149076926</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="2"/>
@@ -2356,7 +3022,7 @@
       </c>
       <c r="L24" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>16.483297294117197</v>
+        <v>10.477282932011112</v>
       </c>
     </row>
     <row r="25" spans="5:12" x14ac:dyDescent="0.3">
@@ -2365,11 +3031,11 @@
       </c>
       <c r="F25" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>2.215109790900089</v>
+        <v>1.4558706647839992</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2915190222171924</v>
+        <v>4.0918529721949097</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="2"/>
@@ -2381,7 +3047,7 @@
       </c>
       <c r="L25" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>7.4897494301758201</v>
+        <v>10.303265336968423</v>
       </c>
     </row>
     <row r="26" spans="5:12" x14ac:dyDescent="0.3">
@@ -2390,11 +3056,11 @@
       </c>
       <c r="F26" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>9.2241642965484179</v>
+        <v>11.108601194817759</v>
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="1"/>
-        <v>7.2018504078749519</v>
+        <v>3.642520471199306</v>
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="2"/>
@@ -2415,23 +3081,23 @@
       </c>
       <c r="F27" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>14.443475283702554</v>
+        <v>2.2439448416324073</v>
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="1"/>
-        <v>4.0143853846785138</v>
+        <v>6.5076798677504</v>
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L27" s="13" t="str">
+        <v>1</v>
+      </c>
+      <c r="L27" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>X</v>
+        <v>18.050648187789491</v>
       </c>
     </row>
     <row r="28" spans="5:12" x14ac:dyDescent="0.3">
@@ -2440,23 +3106,23 @@
       </c>
       <c r="F28" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5054446321900912</v>
+        <v>10.348559635782143</v>
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="1"/>
-        <v>2.0276274702188584</v>
+        <v>3.9311349171008296</v>
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L28" s="13">
+        <v>0</v>
+      </c>
+      <c r="L28" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>24.354286274168224</v>
+        <v>X</v>
       </c>
     </row>
     <row r="29" spans="5:12" x14ac:dyDescent="0.3">
@@ -2465,11 +3131,11 @@
       </c>
       <c r="F29" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28840721702716121</v>
+        <v>12.203379625995739</v>
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="1"/>
-        <v>13.108985321419622</v>
+        <v>8.4036926426714196</v>
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="2"/>
@@ -2477,7 +3143,7 @@
       </c>
       <c r="I29">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L29" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -2490,11 +3156,11 @@
       </c>
       <c r="F30" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>13.942701324553463</v>
+        <v>9.5172924396727314</v>
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="1"/>
-        <v>14.790201411998181</v>
+        <v>4.7020967060367882</v>
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="2"/>
@@ -2515,11 +3181,11 @@
       </c>
       <c r="F31" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>8.0303112626863467</v>
+        <v>15.220625103817618</v>
       </c>
       <c r="G31">
         <f t="shared" ca="1" si="1"/>
-        <v>12.869130506218749</v>
+        <v>12.369802723117623</v>
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="2"/>
@@ -2540,11 +3206,11 @@
       </c>
       <c r="F32" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>6.3870494801139932</v>
+        <v>3.2430093068106114</v>
       </c>
       <c r="G32">
         <f t="shared" ca="1" si="1"/>
-        <v>0.60287889880008216</v>
+        <v>5.4606489133110401</v>
       </c>
       <c r="H32">
         <f t="shared" ca="1" si="2"/>
@@ -2556,7 +3222,7 @@
       </c>
       <c r="L32" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>42.000158859024594</v>
+        <v>21.438407190682323</v>
       </c>
     </row>
     <row r="33" spans="5:12" x14ac:dyDescent="0.3">
@@ -2565,23 +3231,23 @@
       </c>
       <c r="F33" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>8.7596799154483413</v>
+        <v>14.752666537688714</v>
       </c>
       <c r="G33">
         <f t="shared" ca="1" si="1"/>
-        <v>0.22035543004516656</v>
+        <v>6.1481165585682378</v>
       </c>
       <c r="H33">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I33">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L33" s="13">
+        <v>0</v>
+      </c>
+      <c r="L33" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>77.172703081199401</v>
+        <v>X</v>
       </c>
     </row>
     <row r="34" spans="5:12" x14ac:dyDescent="0.3">
@@ -2590,11 +3256,11 @@
       </c>
       <c r="F34" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>11.37496092322678</v>
+        <v>1.2147791075188135</v>
       </c>
       <c r="G34">
         <f t="shared" ca="1" si="1"/>
-        <v>10.091821502281462</v>
+        <v>12.006189688110698</v>
       </c>
       <c r="H34">
         <f t="shared" ca="1" si="2"/>
@@ -2602,7 +3268,7 @@
       </c>
       <c r="I34">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L34" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -2615,23 +3281,23 @@
       </c>
       <c r="F35" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>10.589240736202552</v>
+        <v>0.81872888776665931</v>
       </c>
       <c r="G35">
         <f t="shared" ca="1" si="1"/>
-        <v>5.884461630723627</v>
+        <v>6.4754584160345381</v>
       </c>
       <c r="H35">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L35" s="13" t="str">
+        <v>1</v>
+      </c>
+      <c r="L35" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>X</v>
+        <v>13.621233823732707</v>
       </c>
     </row>
     <row r="36" spans="5:12" x14ac:dyDescent="0.3">
@@ -2640,11 +3306,11 @@
       </c>
       <c r="F36" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>8.2856829962581315</v>
+        <v>6.6058964733651919</v>
       </c>
       <c r="G36">
         <f t="shared" ca="1" si="1"/>
-        <v>6.6830699970841305</v>
+        <v>10.929061768125516</v>
       </c>
       <c r="H36">
         <f t="shared" ca="1" si="2"/>
@@ -2665,23 +3331,23 @@
       </c>
       <c r="F37" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>3.0001465031774432</v>
+        <v>10.543398256248999</v>
       </c>
       <c r="G37">
         <f t="shared" ca="1" si="1"/>
-        <v>6.5133307074991444</v>
+        <v>11.18652335044275</v>
       </c>
       <c r="H37">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I37">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L37" s="13">
+        <v>0</v>
+      </c>
+      <c r="L37" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>22.027540455526129</v>
+        <v>X</v>
       </c>
     </row>
     <row r="38" spans="5:12" x14ac:dyDescent="0.3">
@@ -2690,23 +3356,23 @@
       </c>
       <c r="F38" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>10.349575454356469</v>
+        <v>2.2718083665547146</v>
       </c>
       <c r="G38">
         <f t="shared" ca="1" si="1"/>
-        <v>7.6869447803579103</v>
+        <v>5.6466299179318833</v>
       </c>
       <c r="H38">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I38">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L38" s="13" t="str">
+        <v>1</v>
+      </c>
+      <c r="L38" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>X</v>
+        <v>16.454373090211767</v>
       </c>
     </row>
     <row r="39" spans="5:12" x14ac:dyDescent="0.3">
@@ -2715,11 +3381,11 @@
       </c>
       <c r="F39" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>12.194471627401915</v>
+        <v>8.1955526770526674</v>
       </c>
       <c r="G39">
         <f t="shared" ca="1" si="1"/>
-        <v>13.957626283583696</v>
+        <v>14.924094790329375</v>
       </c>
       <c r="H39">
         <f t="shared" ca="1" si="2"/>
@@ -2740,11 +3406,11 @@
       </c>
       <c r="F40" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4375787861542282</v>
+        <v>11.735660299305781</v>
       </c>
       <c r="G40">
         <f t="shared" ca="1" si="1"/>
-        <v>13.732975247713735</v>
+        <v>5.2020326070127831</v>
       </c>
       <c r="H40">
         <f t="shared" ca="1" si="2"/>
@@ -2765,23 +3431,23 @@
       </c>
       <c r="F41" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.31386002213484587</v>
+        <v>1.2921200388105563</v>
       </c>
       <c r="G41">
         <f t="shared" ca="1" si="1"/>
-        <v>14.80702746110215</v>
+        <v>5.1540000279352896</v>
       </c>
       <c r="H41">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I41">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L41" s="13" t="str">
+        <v>1</v>
+      </c>
+      <c r="L41" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>X</v>
+        <v>11.977574250566372</v>
       </c>
     </row>
     <row r="42" spans="5:12" x14ac:dyDescent="0.3">
@@ -2790,23 +3456,23 @@
       </c>
       <c r="F42" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1262692373430419</v>
+        <v>5.6050471580680954</v>
       </c>
       <c r="G42">
         <f t="shared" ca="1" si="1"/>
-        <v>14.19442178221386</v>
+        <v>0.72386543972576711</v>
       </c>
       <c r="H42">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I42">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L42" s="13" t="str">
+        <v>1</v>
+      </c>
+      <c r="L42" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>X</v>
+        <v>32.864284523618771</v>
       </c>
     </row>
     <row r="43" spans="5:12" x14ac:dyDescent="0.3">
@@ -2815,11 +3481,11 @@
       </c>
       <c r="F43" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>10.492134405157872</v>
+        <v>7.677520804272679</v>
       </c>
       <c r="G43">
         <f t="shared" ca="1" si="1"/>
-        <v>12.029708948889086</v>
+        <v>10.142637766276669</v>
       </c>
       <c r="H43">
         <f t="shared" ca="1" si="2"/>
@@ -2840,11 +3506,11 @@
       </c>
       <c r="F44" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>6.5481651105964627</v>
+        <v>15.204744825897933</v>
       </c>
       <c r="G44">
         <f t="shared" ca="1" si="1"/>
-        <v>5.6151878626315073</v>
+        <v>14.698031075012615</v>
       </c>
       <c r="H44">
         <f t="shared" ca="1" si="2"/>
@@ -2865,15 +3531,15 @@
       </c>
       <c r="F45" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>13.405851014345792</v>
+        <v>10.888018928230569</v>
       </c>
       <c r="G45">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0994276195961949</v>
+        <v>4.949853124301872</v>
       </c>
       <c r="H45">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45">
         <f t="shared" ca="1" si="3"/>
@@ -2890,11 +3556,11 @@
       </c>
       <c r="F46" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1643975964953808</v>
+        <v>5.386875979375044</v>
       </c>
       <c r="G46">
         <f t="shared" ca="1" si="1"/>
-        <v>4.1275510219740212</v>
+        <v>1.7667445297106921</v>
       </c>
       <c r="H46">
         <f t="shared" ca="1" si="2"/>
@@ -2906,7 +3572,7 @@
       </c>
       <c r="L46" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>9.6109238066722611</v>
+        <v>32.551921876589219</v>
       </c>
     </row>
     <row r="47" spans="5:12" x14ac:dyDescent="0.3">
@@ -2915,11 +3581,11 @@
       </c>
       <c r="F47" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1940494933501222</v>
+        <v>13.760836186502662</v>
       </c>
       <c r="G47">
         <f t="shared" ca="1" si="1"/>
-        <v>6.4749737512202117</v>
+        <v>9.3504383989468476</v>
       </c>
       <c r="H47">
         <f t="shared" ca="1" si="2"/>
@@ -2927,7 +3593,7 @@
       </c>
       <c r="I47">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L47" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -2940,11 +3606,11 @@
       </c>
       <c r="F48" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>14.002552984677761</v>
+        <v>15.794652489283319</v>
       </c>
       <c r="G48">
         <f t="shared" ca="1" si="1"/>
-        <v>11.185610271304201</v>
+        <v>1.7698402915787055</v>
       </c>
       <c r="H48">
         <f t="shared" ca="1" si="2"/>
@@ -2965,11 +3631,11 @@
       </c>
       <c r="F49" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>5.3402720514754334</v>
+        <v>2.7908479508962798</v>
       </c>
       <c r="G49">
         <f t="shared" ca="1" si="1"/>
-        <v>8.8566778043109409</v>
+        <v>11.412642370510415</v>
       </c>
       <c r="H49">
         <f t="shared" ca="1" si="2"/>
@@ -2990,23 +3656,23 @@
       </c>
       <c r="F50" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>6.4673689497915827</v>
+        <v>0.16866166645327557</v>
       </c>
       <c r="G50">
         <f t="shared" ca="1" si="1"/>
-        <v>7.6435211780033701</v>
+        <v>7.5669484085603571</v>
       </c>
       <c r="H50">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I50">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L50" s="13" t="str">
+        <v>1</v>
+      </c>
+      <c r="L50" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>X</v>
+        <v>15.16234357485151</v>
       </c>
     </row>
     <row r="51" spans="5:12" x14ac:dyDescent="0.3">
@@ -3015,23 +3681,23 @@
       </c>
       <c r="F51" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>13.098655712086895</v>
+        <v>2.4230996916671295</v>
       </c>
       <c r="G51">
         <f t="shared" ca="1" si="1"/>
-        <v>13.793728552742309</v>
+        <v>7.3232566954982721</v>
       </c>
       <c r="H51">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I51">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L51" s="13" t="str">
+        <v>1</v>
+      </c>
+      <c r="L51" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>X</v>
+        <v>20.517925506753883</v>
       </c>
     </row>
     <row r="52" spans="5:12" x14ac:dyDescent="0.3">
@@ -3040,11 +3706,11 @@
       </c>
       <c r="F52" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.67510880752838265</v>
+        <v>14.458751386411835</v>
       </c>
       <c r="G52">
         <f t="shared" ca="1" si="1"/>
-        <v>8.8865856958201128</v>
+        <v>5.1455877961420979</v>
       </c>
       <c r="H52">
         <f t="shared" ca="1" si="2"/>
@@ -3052,7 +3718,7 @@
       </c>
       <c r="I52">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L52" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -3065,11 +3731,11 @@
       </c>
       <c r="F53" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>6.7922113316548103</v>
+        <v>8.7351163864691639</v>
       </c>
       <c r="G53">
         <f t="shared" ca="1" si="1"/>
-        <v>9.7820147997924742</v>
+        <v>8.7408624893543383</v>
       </c>
       <c r="H53">
         <f t="shared" ca="1" si="2"/>
@@ -3090,11 +3756,11 @@
       </c>
       <c r="F54" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>15.351579761123871</v>
+        <v>16.565655453222551</v>
       </c>
       <c r="G54">
         <f t="shared" ca="1" si="1"/>
-        <v>13.149702738943398</v>
+        <v>8.6769939912137968</v>
       </c>
       <c r="H54">
         <f t="shared" ca="1" si="2"/>
@@ -3115,11 +3781,11 @@
       </c>
       <c r="F55" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2883501238122275</v>
+        <v>6.7759606447768537</v>
       </c>
       <c r="G55">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1910880696097688</v>
+        <v>2.4013542082410515</v>
       </c>
       <c r="H55">
         <f t="shared" ca="1" si="2"/>
@@ -3131,7 +3797,7 @@
       </c>
       <c r="L55" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>7.6187224283709742</v>
+        <v>50.716351076046863</v>
       </c>
     </row>
     <row r="56" spans="5:12" x14ac:dyDescent="0.3">
@@ -3140,23 +3806,23 @@
       </c>
       <c r="F56" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>4.331039556190893</v>
+        <v>5.1224976359130112</v>
       </c>
       <c r="G56">
         <f t="shared" ca="1" si="1"/>
-        <v>9.0017577049781465</v>
+        <v>0.88804780212429102</v>
       </c>
       <c r="H56">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I56">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L56" s="13" t="str">
+        <v>1</v>
+      </c>
+      <c r="L56" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>X</v>
+        <v>28.01607763418297</v>
       </c>
     </row>
     <row r="57" spans="5:12" x14ac:dyDescent="0.3">
@@ -3165,23 +3831,23 @@
       </c>
       <c r="F57" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>2.7275992148315731</v>
+        <v>6.3434247697968695</v>
       </c>
       <c r="G57">
         <f t="shared" ca="1" si="1"/>
-        <v>11.948489902118672</v>
+        <v>3.0702273318709512</v>
       </c>
       <c r="H57">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I57">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L57" s="13" t="str">
+        <v>1</v>
+      </c>
+      <c r="L57" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>X</v>
+        <v>46.379492473814366</v>
       </c>
     </row>
     <row r="58" spans="5:12" x14ac:dyDescent="0.3">
@@ -3190,23 +3856,23 @@
       </c>
       <c r="F58" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>15.030174135796782</v>
+        <v>1.1683609236046597</v>
       </c>
       <c r="G58">
         <f t="shared" ca="1" si="1"/>
-        <v>12.898737226854248</v>
+        <v>5.7788728790605282</v>
       </c>
       <c r="H58">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I58">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L58" s="13" t="str">
+        <v>1</v>
+      </c>
+      <c r="L58" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>X</v>
+        <v>12.92281300592739</v>
       </c>
     </row>
     <row r="59" spans="5:12" x14ac:dyDescent="0.3">
@@ -3215,11 +3881,11 @@
       </c>
       <c r="F59" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>10.975036654223345</v>
+        <v>0.52454286959886132</v>
       </c>
       <c r="G59">
         <f t="shared" ca="1" si="1"/>
-        <v>5.9435017925910918</v>
+        <v>12.271177213451375</v>
       </c>
       <c r="H59">
         <f t="shared" ca="1" si="2"/>
@@ -3227,7 +3893,7 @@
       </c>
       <c r="I59">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L59" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -3240,11 +3906,11 @@
       </c>
       <c r="F60" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>17.399651842161333</v>
+        <v>4.5050051778436595</v>
       </c>
       <c r="G60">
         <f t="shared" ca="1" si="1"/>
-        <v>12.84477441729425</v>
+        <v>8.1173341953627105</v>
       </c>
       <c r="H60">
         <f t="shared" ca="1" si="2"/>
@@ -3252,7 +3918,7 @@
       </c>
       <c r="I60">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L60" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -3265,23 +3931,23 @@
       </c>
       <c r="F61" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11685542398353177</v>
+        <v>16.898975888882937</v>
       </c>
       <c r="G61">
         <f t="shared" ca="1" si="1"/>
-        <v>5.0797029098340198</v>
+        <v>3.4439023779191063</v>
       </c>
       <c r="H61">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I61">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L61" s="13">
+        <v>0</v>
+      </c>
+      <c r="L61" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>10.17306100978241</v>
+        <v>X</v>
       </c>
     </row>
     <row r="62" spans="5:12" x14ac:dyDescent="0.3">
@@ -3290,15 +3956,15 @@
       </c>
       <c r="F62" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>14.669045972439447</v>
+        <v>15.880753161753832</v>
       </c>
       <c r="G62">
         <f t="shared" ca="1" si="1"/>
-        <v>6.1039383413618324</v>
+        <v>0.35735644065547523</v>
       </c>
       <c r="H62">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I62">
         <f t="shared" ca="1" si="3"/>
@@ -3315,11 +3981,11 @@
       </c>
       <c r="F63" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>14.330343238681406</v>
+        <v>15.756105529166499</v>
       </c>
       <c r="G63">
         <f t="shared" ca="1" si="1"/>
-        <v>4.2730511888216371</v>
+        <v>11.171332588040162</v>
       </c>
       <c r="H63">
         <f t="shared" ca="1" si="2"/>
@@ -3340,15 +4006,15 @@
       </c>
       <c r="F64" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>17.114630317721712</v>
+        <v>11.38696101407106</v>
       </c>
       <c r="G64">
         <f t="shared" ca="1" si="1"/>
-        <v>8.4362513289778303</v>
+        <v>0.87753597305551601</v>
       </c>
       <c r="H64">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I64">
         <f t="shared" ca="1" si="3"/>
@@ -3365,11 +4031,11 @@
       </c>
       <c r="F65" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>17.276862436799703</v>
+        <v>4.4044071840749135</v>
       </c>
       <c r="G65">
         <f t="shared" ca="1" si="1"/>
-        <v>0.6513754311601383</v>
+        <v>11.113172007779806</v>
       </c>
       <c r="H65">
         <f t="shared" ca="1" si="2"/>
@@ -3390,23 +4056,23 @@
       </c>
       <c r="F66" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>6.3395589404804102</v>
+        <v>8.4418875909093707</v>
       </c>
       <c r="G66">
         <f t="shared" ca="1" si="1"/>
-        <v>0.36043444022233528</v>
+        <v>9.392602977119985</v>
       </c>
       <c r="H66">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I66">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L66" s="13">
+        <v>0</v>
+      </c>
+      <c r="L66" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>40.910876440269774</v>
+        <v>X</v>
       </c>
     </row>
     <row r="67" spans="5:12" x14ac:dyDescent="0.3">
@@ -3415,23 +4081,23 @@
       </c>
       <c r="F67" s="12">
         <f t="shared" ref="F67:F101" ca="1" si="5">RAND()*17.5</f>
-        <v>17.065213330220367</v>
+        <v>5.7037452970689957</v>
       </c>
       <c r="G67">
         <f t="shared" ref="G67:G101" ca="1" si="6">RAND()*15</f>
-        <v>13.729402306473176</v>
+        <v>3.0217005660592378</v>
       </c>
       <c r="H67">
         <f t="shared" ref="H67:H101" ca="1" si="7">IF(2*F67+4*G67&lt;=35,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I67">
         <f t="shared" ref="I67:I101" ca="1" si="8">IF(3*F67+2*G67&lt;=30,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="L67" s="13" t="str">
+        <v>1</v>
+      </c>
+      <c r="L67" s="13">
         <f t="shared" ref="L67:L101" ca="1" si="9">IF(H67*I67=1,F67^2+2*G67,"X")</f>
-        <v>X</v>
+        <v>38.576111545955165</v>
       </c>
     </row>
     <row r="68" spans="5:12" x14ac:dyDescent="0.3">
@@ -3440,23 +4106,23 @@
       </c>
       <c r="F68" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>3.3088533878270225</v>
+        <v>14.92939990180095</v>
       </c>
       <c r="G68">
         <f t="shared" ca="1" si="6"/>
-        <v>2.8108556728184126</v>
+        <v>9.8673187960208217</v>
       </c>
       <c r="H68">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I68">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="L68" s="13">
+        <v>0</v>
+      </c>
+      <c r="L68" s="13" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>16.570222087771192</v>
+        <v>X</v>
       </c>
     </row>
     <row r="69" spans="5:12" x14ac:dyDescent="0.3">
@@ -3465,23 +4131,23 @@
       </c>
       <c r="F69" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>0.55939753913499124</v>
+        <v>6.359189531620836</v>
       </c>
       <c r="G69">
         <f t="shared" ca="1" si="6"/>
-        <v>10.583390020402215</v>
+        <v>1.4958761300764134</v>
       </c>
       <c r="H69">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I69">
         <f t="shared" ca="1" si="8"/>
         <v>1</v>
       </c>
-      <c r="L69" s="13" t="str">
+      <c r="L69" s="13">
         <f t="shared" ca="1" si="9"/>
-        <v>X</v>
+        <v>43.431043759228857</v>
       </c>
     </row>
     <row r="70" spans="5:12" x14ac:dyDescent="0.3">
@@ -3490,11 +4156,11 @@
       </c>
       <c r="F70" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>4.211912658179501</v>
+        <v>7.6945300535935921</v>
       </c>
       <c r="G70">
         <f t="shared" ca="1" si="6"/>
-        <v>11.133828513225682</v>
+        <v>10.930181549065164</v>
       </c>
       <c r="H70">
         <f t="shared" ca="1" si="7"/>
@@ -3515,23 +4181,23 @@
       </c>
       <c r="F71" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>17.161587043488851</v>
+        <v>1.320349605000279</v>
       </c>
       <c r="G71">
         <f t="shared" ca="1" si="6"/>
-        <v>10.263163506438449</v>
+        <v>1.6197994758507543</v>
       </c>
       <c r="H71">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I71">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="L71" s="13" t="str">
+        <v>1</v>
+      </c>
+      <c r="L71" s="13">
         <f t="shared" ca="1" si="9"/>
-        <v>X</v>
+        <v>4.9829220311259013</v>
       </c>
     </row>
     <row r="72" spans="5:12" x14ac:dyDescent="0.3">
@@ -3540,15 +4206,15 @@
       </c>
       <c r="F72" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>10.543104291871565</v>
+        <v>5.4709384394431817</v>
       </c>
       <c r="G72">
         <f t="shared" ca="1" si="6"/>
-        <v>2.8783931664896309</v>
+        <v>12.178892989649366</v>
       </c>
       <c r="H72">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I72">
         <f t="shared" ca="1" si="8"/>
@@ -3565,11 +4231,11 @@
       </c>
       <c r="F73" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>8.4103985310962095</v>
+        <v>15.149936610598525</v>
       </c>
       <c r="G73">
         <f t="shared" ca="1" si="6"/>
-        <v>8.1853676313898891</v>
+        <v>3.8219702311477173</v>
       </c>
       <c r="H73">
         <f t="shared" ca="1" si="7"/>
@@ -3590,11 +4256,11 @@
       </c>
       <c r="F74" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>6.6644132543030734</v>
+        <v>12.720455259238486</v>
       </c>
       <c r="G74">
         <f t="shared" ca="1" si="6"/>
-        <v>1.6429438561956551</v>
+        <v>1.1494637362586553</v>
       </c>
       <c r="H74">
         <f t="shared" ca="1" si="7"/>
@@ -3602,11 +4268,11 @@
       </c>
       <c r="I74">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="L74" s="13">
+        <v>0</v>
+      </c>
+      <c r="L74" s="13" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>47.700291736521791</v>
+        <v>X</v>
       </c>
     </row>
     <row r="75" spans="5:12" x14ac:dyDescent="0.3">
@@ -3615,11 +4281,11 @@
       </c>
       <c r="F75" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>16.307274218919517</v>
+        <v>9.7809115546819303</v>
       </c>
       <c r="G75">
         <f t="shared" ca="1" si="6"/>
-        <v>5.6050147963666923</v>
+        <v>8.5872167144366642</v>
       </c>
       <c r="H75">
         <f t="shared" ca="1" si="7"/>
@@ -3640,11 +4306,11 @@
       </c>
       <c r="F76" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>2.3928566970321885</v>
+        <v>15.2589159878969</v>
       </c>
       <c r="G76">
         <f t="shared" ca="1" si="6"/>
-        <v>13.07488825620853</v>
+        <v>8.8606398912558237</v>
       </c>
       <c r="H76">
         <f t="shared" ca="1" si="7"/>
@@ -3665,11 +4331,11 @@
       </c>
       <c r="F77" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>9.5310580788794272</v>
+        <v>10.101778172189944</v>
       </c>
       <c r="G77">
         <f t="shared" ca="1" si="6"/>
-        <v>11.016844904723243</v>
+        <v>8.0598171530420402</v>
       </c>
       <c r="H77">
         <f t="shared" ca="1" si="7"/>
@@ -3690,11 +4356,11 @@
       </c>
       <c r="F78" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>16.266290698897894</v>
+        <v>10.968207192932672</v>
       </c>
       <c r="G78">
         <f t="shared" ca="1" si="6"/>
-        <v>8.0169811859397182</v>
+        <v>3.8734992244030431</v>
       </c>
       <c r="H78">
         <f t="shared" ca="1" si="7"/>
@@ -3715,11 +4381,11 @@
       </c>
       <c r="F79" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>17.255163670442236</v>
+        <v>2.0958540728536805</v>
       </c>
       <c r="G79">
         <f t="shared" ca="1" si="6"/>
-        <v>3.4513776252313413</v>
+        <v>8.8101897352607139</v>
       </c>
       <c r="H79">
         <f t="shared" ca="1" si="7"/>
@@ -3727,7 +4393,7 @@
       </c>
       <c r="I79">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L79" s="13" t="str">
         <f t="shared" ca="1" si="9"/>
@@ -3740,11 +4406,11 @@
       </c>
       <c r="F80" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>5.0313969612790084</v>
+        <v>11.613600197679503</v>
       </c>
       <c r="G80">
         <f t="shared" ca="1" si="6"/>
-        <v>14.674100928753456</v>
+        <v>8.1628687553778452</v>
       </c>
       <c r="H80">
         <f t="shared" ca="1" si="7"/>
@@ -3765,11 +4431,11 @@
       </c>
       <c r="F81" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>6.2330162113015088</v>
+        <v>0.51596254943329112</v>
       </c>
       <c r="G81">
         <f t="shared" ca="1" si="6"/>
-        <v>11.614697973819016</v>
+        <v>12.161636261289392</v>
       </c>
       <c r="H81">
         <f t="shared" ca="1" si="7"/>
@@ -3777,7 +4443,7 @@
       </c>
       <c r="I81">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L81" s="13" t="str">
         <f t="shared" ca="1" si="9"/>
@@ -3790,15 +4456,15 @@
       </c>
       <c r="F82" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>12.149102659775647</v>
+        <v>12.064789099647287</v>
       </c>
       <c r="G82">
         <f t="shared" ca="1" si="6"/>
-        <v>12.574376045197152</v>
+        <v>0.89414919764739476</v>
       </c>
       <c r="H82">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I82">
         <f t="shared" ca="1" si="8"/>
@@ -3815,23 +4481,23 @@
       </c>
       <c r="F83" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>4.2311509169723953</v>
+        <v>11.244725263340982</v>
       </c>
       <c r="G83">
         <f t="shared" ca="1" si="6"/>
-        <v>0.4109764515403358</v>
+        <v>10.147157063418073</v>
       </c>
       <c r="H83">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I83">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="L83" s="13">
+        <v>0</v>
+      </c>
+      <c r="L83" s="13" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>18.724590985277011</v>
+        <v>X</v>
       </c>
     </row>
     <row r="84" spans="5:12" x14ac:dyDescent="0.3">
@@ -3840,11 +4506,11 @@
       </c>
       <c r="F84" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>12.38187385613532</v>
+        <v>11.216823294491579</v>
       </c>
       <c r="G84">
         <f t="shared" ca="1" si="6"/>
-        <v>13.183893943326174</v>
+        <v>6.5054106080305312</v>
       </c>
       <c r="H84">
         <f t="shared" ca="1" si="7"/>
@@ -3865,11 +4531,11 @@
       </c>
       <c r="F85" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>13.539320892435638</v>
+        <v>1.7146662872402743</v>
       </c>
       <c r="G85">
         <f t="shared" ca="1" si="6"/>
-        <v>5.022299500863185</v>
+        <v>8.9148309373022894</v>
       </c>
       <c r="H85">
         <f t="shared" ca="1" si="7"/>
@@ -3877,7 +4543,7 @@
       </c>
       <c r="I85">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L85" s="13" t="str">
         <f t="shared" ca="1" si="9"/>
@@ -3890,11 +4556,11 @@
       </c>
       <c r="F86" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>17.115153517372551</v>
+        <v>11.764065937942787</v>
       </c>
       <c r="G86">
         <f t="shared" ca="1" si="6"/>
-        <v>13.747496343024492</v>
+        <v>13.807245007001743</v>
       </c>
       <c r="H86">
         <f t="shared" ca="1" si="7"/>
@@ -3915,11 +4581,11 @@
       </c>
       <c r="F87" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>14.863602952083768</v>
+        <v>8.4263640504329942</v>
       </c>
       <c r="G87">
         <f t="shared" ca="1" si="6"/>
-        <v>5.7387518361750249</v>
+        <v>8.3778425949015265</v>
       </c>
       <c r="H87">
         <f t="shared" ca="1" si="7"/>
@@ -3940,11 +4606,11 @@
       </c>
       <c r="F88" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>10.485779171082207</v>
+        <v>14.0973053588126</v>
       </c>
       <c r="G88">
         <f t="shared" ca="1" si="6"/>
-        <v>11.421925560732157</v>
+        <v>5.3287383279185967</v>
       </c>
       <c r="H88">
         <f t="shared" ca="1" si="7"/>
@@ -3965,11 +4631,11 @@
       </c>
       <c r="F89" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>13.34723288122709</v>
+        <v>9.718002326440212</v>
       </c>
       <c r="G89">
         <f t="shared" ca="1" si="6"/>
-        <v>12.199995758289292</v>
+        <v>10.202275973905911</v>
       </c>
       <c r="H89">
         <f t="shared" ca="1" si="7"/>
@@ -3990,11 +4656,11 @@
       </c>
       <c r="F90" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>8.4902615423532524</v>
+        <v>9.9060999159675855</v>
       </c>
       <c r="G90">
         <f t="shared" ca="1" si="6"/>
-        <v>10.015327458706791</v>
+        <v>14.859683053388462</v>
       </c>
       <c r="H90">
         <f t="shared" ca="1" si="7"/>
@@ -4015,11 +4681,11 @@
       </c>
       <c r="F91" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>6.6703502482542314</v>
+        <v>5.2554502002019436</v>
       </c>
       <c r="G91">
         <f t="shared" ca="1" si="6"/>
-        <v>12.648008090856379</v>
+        <v>11.597329862628778</v>
       </c>
       <c r="H91">
         <f t="shared" ca="1" si="7"/>
@@ -4040,11 +4706,11 @@
       </c>
       <c r="F92" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>13.544381809418178</v>
+        <v>11.781443145761159</v>
       </c>
       <c r="G92">
         <f t="shared" ca="1" si="6"/>
-        <v>9.308442809675638</v>
+        <v>6.2370569693374813</v>
       </c>
       <c r="H92">
         <f t="shared" ca="1" si="7"/>
@@ -4065,23 +4731,23 @@
       </c>
       <c r="F93" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>12.439876009800344</v>
+        <v>3.8965797875712913</v>
       </c>
       <c r="G93">
         <f t="shared" ca="1" si="6"/>
-        <v>10.166106929561844</v>
+        <v>3.1298359405252061</v>
       </c>
       <c r="H93">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I93">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="L93" s="13" t="str">
+        <v>1</v>
+      </c>
+      <c r="L93" s="13">
         <f t="shared" ca="1" si="9"/>
-        <v>X</v>
+        <v>21.443005921959539</v>
       </c>
     </row>
     <row r="94" spans="5:12" x14ac:dyDescent="0.3">
@@ -4090,11 +4756,11 @@
       </c>
       <c r="F94" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>17.044930711371503</v>
+        <v>4.8981277648654959</v>
       </c>
       <c r="G94">
         <f t="shared" ca="1" si="6"/>
-        <v>6.8275571251634037</v>
+        <v>10.99202244962262</v>
       </c>
       <c r="H94">
         <f t="shared" ca="1" si="7"/>
@@ -4115,23 +4781,23 @@
       </c>
       <c r="F95" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>9.9680300855040063</v>
+        <v>0.86056569189825793</v>
       </c>
       <c r="G95">
         <f t="shared" ca="1" si="6"/>
-        <v>13.116529713976282</v>
+        <v>5.9633624884656999</v>
       </c>
       <c r="H95">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I95">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="L95" s="13" t="str">
+        <v>1</v>
+      </c>
+      <c r="L95" s="13">
         <f t="shared" ca="1" si="9"/>
-        <v>X</v>
+        <v>12.667298287003728</v>
       </c>
     </row>
     <row r="96" spans="5:12" x14ac:dyDescent="0.3">
@@ -4140,23 +4806,23 @@
       </c>
       <c r="F96" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>1.1173066843994326</v>
+        <v>12.11154787986321</v>
       </c>
       <c r="G96">
         <f t="shared" ca="1" si="6"/>
-        <v>1.7426104564438845</v>
+        <v>10.802678051718456</v>
       </c>
       <c r="H96">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I96">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="L96" s="13">
+        <v>0</v>
+      </c>
+      <c r="L96" s="13" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>4.7335951398914222</v>
+        <v>X</v>
       </c>
     </row>
     <row r="97" spans="5:12" x14ac:dyDescent="0.3">
@@ -4165,11 +4831,11 @@
       </c>
       <c r="F97" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>7.9276794767552232</v>
+        <v>13.296066306466825</v>
       </c>
       <c r="G97">
         <f t="shared" ca="1" si="6"/>
-        <v>10.045619572366537</v>
+        <v>14.525536717624126</v>
       </c>
       <c r="H97">
         <f t="shared" ca="1" si="7"/>
@@ -4190,11 +4856,11 @@
       </c>
       <c r="F98" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>12.672877351297503</v>
+        <v>15.787395278957087</v>
       </c>
       <c r="G98">
         <f t="shared" ca="1" si="6"/>
-        <v>7.3212463708839906</v>
+        <v>7.0629840477258945</v>
       </c>
       <c r="H98">
         <f t="shared" ca="1" si="7"/>
@@ -4215,11 +4881,11 @@
       </c>
       <c r="F99" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>10.485917452414355</v>
+        <v>5.1595584655409761</v>
       </c>
       <c r="G99">
         <f t="shared" ca="1" si="6"/>
-        <v>6.9726675058145373</v>
+        <v>6.1972332461546156</v>
       </c>
       <c r="H99">
         <f t="shared" ca="1" si="7"/>
@@ -4227,7 +4893,7 @@
       </c>
       <c r="I99">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L99" s="13" t="str">
         <f t="shared" ca="1" si="9"/>
@@ -4240,11 +4906,11 @@
       </c>
       <c r="F100" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>8.0997494630142519</v>
+        <v>12.070793849837315</v>
       </c>
       <c r="G100">
         <f t="shared" ca="1" si="6"/>
-        <v>4.9520379544110815</v>
+        <v>10.967908641792262</v>
       </c>
       <c r="H100">
         <f t="shared" ca="1" si="7"/>
@@ -4265,23 +4931,23 @@
       </c>
       <c r="F101" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>16.105773370993973</v>
+        <v>1.9172621267829626</v>
       </c>
       <c r="G101">
         <f t="shared" ca="1" si="6"/>
-        <v>8.7668336307225374</v>
+        <v>4.2495365611545139</v>
       </c>
       <c r="H101">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I101">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="L101" s="13" t="str">
+        <v>1</v>
+      </c>
+      <c r="L101" s="13">
         <f t="shared" ca="1" si="9"/>
-        <v>X</v>
+        <v>12.174967185105357</v>
       </c>
     </row>
     <row r="102" spans="5:12" x14ac:dyDescent="0.3">
@@ -6883,6 +7549,87 @@
     <row r="751" spans="6:12" x14ac:dyDescent="0.3">
       <c r="F751" s="12"/>
       <c r="L751" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AAABCF8-759C-4405-B0A6-BE54EFF7A346}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="10">
+        <f>D3^2+3*E3</f>
+        <v>26.25</v>
+      </c>
+      <c r="D3" s="10">
+        <v>0</v>
+      </c>
+      <c r="E3" s="10">
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4">
+        <f>2*D3+4*E3</f>
+        <v>35</v>
+      </c>
+      <c r="D4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5">
+        <f>3*D3+2*E3</f>
+        <v>17.5</v>
+      </c>
+      <c r="D5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>